<commit_message>
change docker, first Azure beta test
</commit_message>
<xml_diff>
--- a/uploads/mantencibnsad.xlsx
+++ b/uploads/mantencibnsad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konko\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14DADB2-6B91-41F7-9C1E-59CFFCA0CB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0014E9F-85A4-45E0-BDC4-78ACDECF7803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2214,7 +2214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2314,7 +2314,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2598,8 +2597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L453"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C453" sqref="C453"/>
+    <sheetView tabSelected="1" topLeftCell="A222" zoomScale="80" workbookViewId="0">
+      <selection activeCell="B241" sqref="B241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2614,7 +2613,7 @@
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="123.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="131.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -14668,7 +14667,7 @@
       <c r="B385" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C385" s="51" t="s">
+      <c r="C385" s="45" t="s">
         <v>664</v>
       </c>
       <c r="D385" s="46">

</xml_diff>